<commit_message>
changes as per 31st 2017
</commit_message>
<xml_diff>
--- a/Silver Inventory Doc/Silver Database Design.xlsx
+++ b/Silver Inventory Doc/Silver Database Design.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Disk 2\silver_git\silver\Silver Inventory Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Git_Silver\silver\Silver Inventory Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="7530" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="7530" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Entity" sheetId="1" r:id="rId1"/>
     <sheet name="Transactions" sheetId="2" r:id="rId2"/>
     <sheet name="ER Diagram" sheetId="5" r:id="rId3"/>
-    <sheet name="Report" sheetId="3" r:id="rId4"/>
-    <sheet name="Example" sheetId="4" r:id="rId5"/>
-    <sheet name="TimeLine" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId4"/>
+    <sheet name="Report" sheetId="3" r:id="rId5"/>
+    <sheet name="Example" sheetId="4" r:id="rId6"/>
+    <sheet name="TimeLine" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="202">
   <si>
     <t>Silver</t>
   </si>
@@ -612,12 +613,36 @@
   </si>
   <si>
     <t>your order is ready to pickup</t>
+  </si>
+  <si>
+    <t>Transaction type</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>OUT</t>
+  </si>
+  <si>
+    <t>MOBILE</t>
+  </si>
+  <si>
+    <t>Search</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1041,7 +1066,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -1084,6 +1109,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1093,9 +1121,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1504,7 +1530,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="21" formatCode="dd\-mmm"/>
+      <numFmt numFmtId="164" formatCode="dd\-mmm"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1735,7 +1761,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="21" formatCode="dd\-mmm"/>
+      <numFmt numFmtId="164" formatCode="dd\-mmm"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1829,7 +1855,7 @@
         <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41C739B8-841D-4DF6-A220-AA9C7CD9CDAA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41C739B8-841D-4DF6-A220-AA9C7CD9CDAA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1882,7 +1908,7 @@
         <xdr:cNvPr id="10" name="Connector: Elbow 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD2556BA-ADA4-44AC-85F9-67BB72CB0F38}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD2556BA-ADA4-44AC-85F9-67BB72CB0F38}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1938,7 +1964,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F16D2EBA-661D-4756-8F53-88D5A741A643}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F16D2EBA-661D-4756-8F53-88D5A741A643}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2362,11 +2388,11 @@
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="39"/>
-      <c r="F1" s="40"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2519,8 +2545,8 @@
   </sheetPr>
   <dimension ref="A2:AC33"/>
   <sheetViews>
-    <sheetView topLeftCell="E6" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView topLeftCell="H20" workbookViewId="0">
+      <selection activeCell="U42" sqref="U42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3199,8 +3225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:Y53"/>
   <sheetViews>
-    <sheetView topLeftCell="J28" workbookViewId="0">
-      <selection activeCell="P46" sqref="P46"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3214,7 +3240,7 @@
     <col min="8" max="8" width="13.7109375" customWidth="1"/>
     <col min="9" max="9" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.28515625" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" customWidth="1"/>
     <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="11" customWidth="1"/>
@@ -3480,6 +3506,9 @@
       <c r="G21" s="3" t="s">
         <v>123</v>
       </c>
+      <c r="K21" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="22" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F22" s="3" t="s">
@@ -3488,6 +3517,15 @@
       <c r="G22" s="3" t="s">
         <v>124</v>
       </c>
+      <c r="K22" t="s">
+        <v>29</v>
+      </c>
+      <c r="L22" t="s">
+        <v>66</v>
+      </c>
+      <c r="M22" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="23" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F23" s="3" t="s">
@@ -3496,6 +3534,15 @@
       <c r="G23" s="3" t="s">
         <v>125</v>
       </c>
+      <c r="K23" t="s">
+        <v>28</v>
+      </c>
+      <c r="L23" t="s">
+        <v>195</v>
+      </c>
+      <c r="M23" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="24" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F24" s="3" t="s">
@@ -3504,6 +3551,15 @@
       <c r="G24" s="3" t="s">
         <v>125</v>
       </c>
+      <c r="K24" t="s">
+        <v>30</v>
+      </c>
+      <c r="L24" t="s">
+        <v>196</v>
+      </c>
+      <c r="M24" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="25" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F25" s="3" t="s">
@@ -3511,6 +3567,15 @@
       </c>
       <c r="G25" s="3" t="s">
         <v>126</v>
+      </c>
+      <c r="K25" t="s">
+        <v>31</v>
+      </c>
+      <c r="L25" t="s">
+        <v>197</v>
+      </c>
+      <c r="M25" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="26" spans="6:20" x14ac:dyDescent="0.25">
@@ -4266,6 +4331,97 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="44"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="44"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="44"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="44"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="44"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
@@ -4279,7 +4435,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF79DC"/>
@@ -4409,12 +4565,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4425,13 +4581,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="40" t="s">
         <v>182</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="40" t="s">
         <v>185</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="D2" s="40" t="s">
         <v>188</v>
       </c>
     </row>
@@ -4442,7 +4598,7 @@
       <c r="C3" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D3" s="42">
+      <c r="D3" s="39">
         <v>43094</v>
       </c>
     </row>
@@ -4453,7 +4609,7 @@
       <c r="C4" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="D4" s="42">
+      <c r="D4" s="39">
         <v>43093</v>
       </c>
     </row>
@@ -4464,7 +4620,7 @@
       <c r="C5" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="D5" s="42">
+      <c r="D5" s="39">
         <v>43095</v>
       </c>
     </row>
@@ -4475,7 +4631,7 @@
       <c r="C6" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="D6" s="42">
+      <c r="D6" s="39">
         <v>43107</v>
       </c>
     </row>
@@ -4486,7 +4642,7 @@
       <c r="C7" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="D7" s="42">
+      <c r="D7" s="39">
         <v>43107</v>
       </c>
     </row>
@@ -4497,7 +4653,7 @@
       <c r="C8" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D8" s="42">
+      <c r="D8" s="39">
         <v>43094</v>
       </c>
       <c r="J8" t="s">
@@ -4514,12 +4670,12 @@
       <c r="C9" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D9" s="42">
+      <c r="D9" s="39">
         <v>43099</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="38" t="s">
         <v>190</v>
       </c>
       <c r="C10" s="3"/>
@@ -4532,7 +4688,7 @@
       <c r="C11" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D11" s="42">
+      <c r="D11" s="39">
         <v>43107</v>
       </c>
     </row>
@@ -4547,7 +4703,7 @@
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="38" t="s">
         <v>191</v>
       </c>
       <c r="C14" s="3"/>

</xml_diff>